<commit_message>
Added data for 2019 NI europarl votes Signed-off-by: Gerry Mulvenna <git@movingwifi.com>
</commit_message>
<xml_diff>
--- a/europarl/transfers.2019-05-23.xlsx
+++ b/europarl/transfers.2019-05-23.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
   <si>
     <t>Martina Anderson</t>
   </si>
@@ -156,7 +156,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -170,6 +170,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -472,15 +473,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15:J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -502,6 +505,9 @@
       <c r="H1" t="s">
         <v>13</v>
       </c>
+      <c r="I1">
+        <v>62021</v>
+      </c>
       <c r="J1" s="3">
         <v>62021</v>
       </c>
@@ -525,6 +531,9 @@
       <c r="H2" t="s">
         <v>15</v>
       </c>
+      <c r="I2">
+        <v>126951</v>
+      </c>
       <c r="J2" s="3">
         <v>126951</v>
       </c>
@@ -548,6 +557,9 @@
       <c r="H3" t="s">
         <v>16</v>
       </c>
+      <c r="I3">
+        <v>12471</v>
+      </c>
       <c r="J3" s="3">
         <v>12471</v>
       </c>
@@ -571,6 +583,9 @@
       <c r="H4" t="s">
         <v>18</v>
       </c>
+      <c r="I4">
+        <v>662</v>
+      </c>
       <c r="J4" s="2">
         <v>662</v>
       </c>
@@ -594,6 +609,9 @@
       <c r="H5" t="s">
         <v>20</v>
       </c>
+      <c r="I5">
+        <v>124991</v>
+      </c>
       <c r="J5" s="3">
         <v>124991</v>
       </c>
@@ -617,6 +635,9 @@
       <c r="H6" t="s">
         <v>19</v>
       </c>
+      <c r="I6">
+        <v>78589</v>
+      </c>
       <c r="J6" s="3">
         <v>78589</v>
       </c>
@@ -640,6 +661,9 @@
       <c r="H7" t="s">
         <v>17</v>
       </c>
+      <c r="I7">
+        <v>5115</v>
+      </c>
       <c r="J7" s="3">
         <v>5115</v>
       </c>
@@ -663,6 +687,9 @@
       <c r="H8" t="s">
         <v>12</v>
       </c>
+      <c r="I8">
+        <v>53052</v>
+      </c>
       <c r="J8" s="3">
         <v>53052</v>
       </c>
@@ -686,6 +713,9 @@
       <c r="H9" t="s">
         <v>14</v>
       </c>
+      <c r="I9">
+        <v>105928</v>
+      </c>
       <c r="J9" s="3">
         <v>105928</v>
       </c>
@@ -709,6 +739,9 @@
       <c r="H10" t="s">
         <v>22</v>
       </c>
+      <c r="I10">
+        <v>948</v>
+      </c>
       <c r="J10" s="2">
         <v>948</v>
       </c>
@@ -732,9 +765,385 @@
       <c r="H11" t="s">
         <v>21</v>
       </c>
+      <c r="I11">
+        <v>1719</v>
+      </c>
       <c r="J11" s="3">
         <v>1719</v>
       </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>62021</v>
+      </c>
+      <c r="C15">
+        <f>D15-B15</f>
+        <v>1851</v>
+      </c>
+      <c r="D15">
+        <v>63872</v>
+      </c>
+      <c r="E15">
+        <f t="shared" ref="E15:E16" si="0">F15-D15</f>
+        <v>15668</v>
+      </c>
+      <c r="F15">
+        <v>79540</v>
+      </c>
+      <c r="G15">
+        <f t="shared" ref="G15:I16" si="1">H15-F15</f>
+        <v>10314</v>
+      </c>
+      <c r="H15" s="5">
+        <v>89854</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>225</v>
+      </c>
+      <c r="J15" s="5">
+        <v>90079</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>126951</v>
+      </c>
+      <c r="C16">
+        <f>D16-B16</f>
+        <v>1166</v>
+      </c>
+      <c r="D16">
+        <v>128117</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>-927</v>
+      </c>
+      <c r="F16">
+        <v>127190</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>1010.5</v>
+      </c>
+      <c r="H16" s="5">
+        <v>128200.5</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="1"/>
+        <v>24236</v>
+      </c>
+      <c r="J16" s="5">
+        <v>152436.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>12471</v>
+      </c>
+      <c r="C17">
+        <f>-B17</f>
+        <v>-12471</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17" s="5">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>662</v>
+      </c>
+      <c r="C18">
+        <f>-B18</f>
+        <v>-662</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18" s="5">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19">
+        <v>124991</v>
+      </c>
+      <c r="C19">
+        <f>D19-B19</f>
+        <v>2300</v>
+      </c>
+      <c r="D19">
+        <v>127291</v>
+      </c>
+      <c r="E19">
+        <f t="shared" ref="E19:E20" si="2">F19-D19</f>
+        <v>28131</v>
+      </c>
+      <c r="F19">
+        <v>155422</v>
+      </c>
+      <c r="G19">
+        <f>143112-F19</f>
+        <v>-12310</v>
+      </c>
+      <c r="H19" s="5">
+        <v>143112</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19" s="5">
+        <v>143112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>78589</v>
+      </c>
+      <c r="D20">
+        <v>80949</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>1152</v>
+      </c>
+      <c r="F20">
+        <v>82101</v>
+      </c>
+      <c r="G20">
+        <f>H20-F20</f>
+        <v>312.5</v>
+      </c>
+      <c r="H20" s="5">
+        <v>82413.5</v>
+      </c>
+      <c r="I20" s="5">
+        <f>-H20</f>
+        <v>-82413.5</v>
+      </c>
+      <c r="J20" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21">
+        <v>5115</v>
+      </c>
+      <c r="C21">
+        <f>-B21</f>
+        <v>-5115</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21" s="5">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22">
+        <v>53052</v>
+      </c>
+      <c r="D22">
+        <v>53052</v>
+      </c>
+      <c r="E22">
+        <f>-D22</f>
+        <v>-53052</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22" s="5">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23">
+        <v>105928</v>
+      </c>
+      <c r="C23">
+        <f>D23-B23</f>
+        <v>9399</v>
+      </c>
+      <c r="D23">
+        <v>115327</v>
+      </c>
+      <c r="E23">
+        <f>F23-D23</f>
+        <v>6936</v>
+      </c>
+      <c r="F23">
+        <v>122263</v>
+      </c>
+      <c r="G23">
+        <f>H23-F23</f>
+        <v>1654</v>
+      </c>
+      <c r="H23" s="5">
+        <v>123917</v>
+      </c>
+      <c r="I23">
+        <f>J23-H23</f>
+        <v>46453</v>
+      </c>
+      <c r="J23" s="5">
+        <v>170370</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>948</v>
+      </c>
+      <c r="C24">
+        <f>-B24</f>
+        <v>-948</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24" s="5">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25">
+        <v>1719</v>
+      </c>
+      <c r="C25">
+        <f>-B25</f>
+        <v>-1719</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25" s="5">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J26" s="5"/>
     </row>
   </sheetData>
   <sortState ref="E1:H11">

</xml_diff>

<commit_message>
Corrected error in 2019 figures Signed-off-by: Gerry Mulvenna <git@movingwifi.com>
</commit_message>
<xml_diff>
--- a/europarl/transfers.2019-05-23.xlsx
+++ b/europarl/transfers.2019-05-23.xlsx
@@ -475,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:J25"/>
+    <sheetView tabSelected="1" topLeftCell="E10" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -952,6 +952,10 @@
       <c r="B20">
         <v>78589</v>
       </c>
+      <c r="C20">
+        <f>D20-B20</f>
+        <v>2360</v>
+      </c>
       <c r="D20">
         <v>80949</v>
       </c>
@@ -1017,12 +1021,16 @@
       <c r="B22">
         <v>53052</v>
       </c>
+      <c r="C22">
+        <f>D22-B22</f>
+        <v>1684</v>
+      </c>
       <c r="D22">
-        <v>53052</v>
+        <v>54736</v>
       </c>
       <c r="E22">
         <f>-D22</f>
-        <v>-53052</v>
+        <v>-54736</v>
       </c>
       <c r="F22">
         <v>0</v>

</xml_diff>